<commit_message>
Update Excel config handling and cleanup
add features
- Added `LastModified` property to `ExcelConfigResultModel` for tracking the last modification date of Excel config files.
- Updated `ExcelConfigService` to include and sort by `LastModified` in the result set.
- Removed user secrets setup from `App.xaml.cs`, indicating a shift in configuration management.
- Adjusted project file to update handling of Excel configuration files, including changes to file inclusion and exclusion.
- Modified `appsettings.json` to update the default connection string with sensitive information directly and commented out an alternative setup.
</commit_message>
<xml_diff>
--- a/SGS.HN.Labeler.WPF/ExcelConfig/PrintInfo.xlsx
+++ b/SGS.HN.Labeler.WPF/ExcelConfig/PrintInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\SGS.HN.Labeler\SGS.HN.Labeler.WPF\ExcelConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0620EB-01DA-4E69-BF38-B32549B8CC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E85AECD-536E-4160-B60D-F5DD40CE3A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30195" yWindow="2115" windowWidth="25035" windowHeight="13725" xr2:uid="{4B29951C-24DD-4481-B16C-FA382712CE54}"/>
+    <workbookView xWindow="30195" yWindow="1755" windowWidth="25035" windowHeight="13725" xr2:uid="{4B29951C-24DD-4481-B16C-FA382712CE54}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>ID (SL)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>1902_MR-4(植)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>開發測試使用，正式DB無效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需先修改資料庫連線為 LIMS UAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用訂單編號 AVO24200001 或 AVO24100002</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -235,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,8 +284,15 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +384,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -413,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,11 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040A9356-0BF4-4731-8847-4EC52DB9F2BC}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1218,6 +1246,21 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
     </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" sortMethod="pinYin" ref="A2:U11">
     <sortCondition sortBy="cellColor" ref="B2:B11" dxfId="1"/>

</xml_diff>